<commit_message>
translate until cell 41.
</commit_message>
<xml_diff>
--- a/data/gender identity/Data prep/Gender_identity_ShortList_norwegian.xlsx
+++ b/data/gender identity/Data prep/Gender_identity_ShortList_norwegian.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="403">
   <si>
     <t>Categorization</t>
   </si>
@@ -558,9 +558,6 @@
   </si>
   <si>
     <t>A transgendered person and a friend were discussing their recent health challenges.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Who has a mental health diagnosis?</t>
@@ -1298,7 +1295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1317,9 +1314,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1632,7 +1626,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
     <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
     <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
     <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
@@ -1646,7 +1640,7 @@
     <col min="12" max="12" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="3" width="24.719285714285714" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3604,20 +3598,18 @@
       <c r="I42" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J42" s="7" t="s">
+      <c r="J42" s="2"/>
+      <c r="K42" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>167</v>
       </c>
       <c r="M42" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N42" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="N42" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="O42" s="6">
         <v>1</v>
@@ -3649,20 +3641,20 @@
         <v>3</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>167</v>
       </c>
       <c r="M43" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N43" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="N43" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="O43" s="6">
         <v>2</v>
@@ -3685,7 +3677,7 @@
         <v>22</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>179</v>
@@ -3694,17 +3686,17 @@
         <v>3</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>167</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>166</v>
@@ -3730,7 +3722,7 @@
         <v>22</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>179</v>
@@ -3739,17 +3731,17 @@
         <v>3</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>167</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>166</v>
@@ -3763,7 +3755,7 @@
         <v>216</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>20</v>
@@ -3775,29 +3767,29 @@
         <v>22</v>
       </c>
       <c r="F46" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L46" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="M46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N46" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="O46" s="6">
         <v>1</v>
@@ -3808,7 +3800,7 @@
         <v>217</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>20</v>
@@ -3820,29 +3812,29 @@
         <v>22</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="H47" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="M47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N47" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="O47" s="6">
         <v>2</v>
@@ -3853,7 +3845,7 @@
         <v>220</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>20</v>
@@ -3865,26 +3857,26 @@
         <v>22</v>
       </c>
       <c r="F48" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M48" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>107</v>
@@ -3898,7 +3890,7 @@
         <v>221</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>20</v>
@@ -3910,26 +3902,26 @@
         <v>22</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M49" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>107</v>
@@ -3943,7 +3935,7 @@
         <v>280</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>20</v>
@@ -3955,29 +3947,29 @@
         <v>22</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>173</v>
       </c>
       <c r="M50" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="N50" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="N50" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="O50" s="6">
         <v>0</v>
@@ -3988,7 +3980,7 @@
         <v>281</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>20</v>
@@ -4000,29 +3992,29 @@
         <v>22</v>
       </c>
       <c r="F51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="H51" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>173</v>
       </c>
       <c r="M51" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="N51" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="N51" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="O51" s="6">
         <v>2</v>
@@ -4033,7 +4025,7 @@
         <v>284</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>20</v>
@@ -4045,29 +4037,29 @@
         <v>22</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O52" s="6">
         <v>0</v>
@@ -4078,7 +4070,7 @@
         <v>285</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>20</v>
@@ -4090,29 +4082,29 @@
         <v>22</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O53" s="6">
         <v>1</v>
@@ -4123,7 +4115,7 @@
         <v>328</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>20</v>
@@ -4135,20 +4127,20 @@
         <v>22</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H54" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>106</v>
@@ -4168,7 +4160,7 @@
         <v>329</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>20</v>
@@ -4180,20 +4172,20 @@
         <v>22</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>106</v>
@@ -4213,7 +4205,7 @@
         <v>332</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>20</v>
@@ -4231,14 +4223,14 @@
         <v>24</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>114</v>
@@ -4258,7 +4250,7 @@
         <v>333</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>20</v>
@@ -4276,14 +4268,14 @@
         <v>24</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>114</v>
@@ -4303,7 +4295,7 @@
         <v>336</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>20</v>
@@ -4315,26 +4307,26 @@
         <v>22</v>
       </c>
       <c r="F58" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N58" s="2" t="s">
         <v>108</v>
@@ -4348,7 +4340,7 @@
         <v>337</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>20</v>
@@ -4360,26 +4352,26 @@
         <v>22</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="H59" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>108</v>
@@ -4393,7 +4385,7 @@
         <v>340</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>20</v>
@@ -4405,20 +4397,20 @@
         <v>22</v>
       </c>
       <c r="F60" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I60" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>108</v>
@@ -4438,7 +4430,7 @@
         <v>341</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>20</v>
@@ -4450,20 +4442,20 @@
         <v>22</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>108</v>
@@ -4483,7 +4475,7 @@
         <v>344</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>20</v>
@@ -4495,29 +4487,29 @@
         <v>22</v>
       </c>
       <c r="F62" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="H62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="N62" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M62" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="N62" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="O62" s="6">
         <v>2</v>
@@ -4528,7 +4520,7 @@
         <v>345</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>20</v>
@@ -4540,29 +4532,29 @@
         <v>22</v>
       </c>
       <c r="F63" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="H63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="N63" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="N63" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="O63" s="6">
         <v>0</v>
@@ -4573,7 +4565,7 @@
         <v>348</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>20</v>
@@ -4585,29 +4577,29 @@
         <v>22</v>
       </c>
       <c r="F64" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O64" s="6">
         <v>1</v>
@@ -4618,7 +4610,7 @@
         <v>349</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>20</v>
@@ -4630,29 +4622,29 @@
         <v>22</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O65" s="6">
         <v>0</v>
@@ -4663,7 +4655,7 @@
         <v>468</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>20</v>
@@ -4675,29 +4667,29 @@
         <v>22</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I66" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M66" s="2" t="s">
         <v>166</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O66" s="6">
         <v>1</v>
@@ -4708,7 +4700,7 @@
         <v>469</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>20</v>
@@ -4720,29 +4712,29 @@
         <v>22</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="H67" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M67" s="2" t="s">
         <v>166</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O67" s="6">
         <v>0</v>
@@ -4753,7 +4745,7 @@
         <v>472</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>20</v>
@@ -4765,29 +4757,29 @@
         <v>22</v>
       </c>
       <c r="F68" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I68" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M68" s="2" t="s">
         <v>107</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O68" s="6">
         <v>1</v>
@@ -4798,7 +4790,7 @@
         <v>473</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>20</v>
@@ -4810,29 +4802,29 @@
         <v>22</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M69" s="2" t="s">
         <v>107</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O69" s="6">
         <v>2</v>
@@ -4843,7 +4835,7 @@
         <v>476</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>20</v>
@@ -4855,29 +4847,29 @@
         <v>22</v>
       </c>
       <c r="F70" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I70" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M70" s="2" t="s">
         <v>107</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O70" s="6">
         <v>1</v>
@@ -4888,7 +4880,7 @@
         <v>477</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>20</v>
@@ -4900,29 +4892,29 @@
         <v>22</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>107</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O71" s="6">
         <v>0</v>
@@ -4933,7 +4925,7 @@
         <v>596</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>20</v>
@@ -4945,29 +4937,29 @@
         <v>22</v>
       </c>
       <c r="F72" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L72" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N72" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="O72" s="6">
         <v>1</v>
@@ -4978,7 +4970,7 @@
         <v>597</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>20</v>
@@ -4990,29 +4982,29 @@
         <v>22</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L73" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N73" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="N73" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="O73" s="6">
         <v>0</v>
@@ -5023,7 +5015,7 @@
         <v>600</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>20</v>
@@ -5038,23 +5030,23 @@
         <v>23</v>
       </c>
       <c r="G74" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="J74" s="2"/>
       <c r="K74" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N74" s="2" t="s">
         <v>108</v>
@@ -5068,7 +5060,7 @@
         <v>601</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>20</v>
@@ -5083,23 +5075,23 @@
         <v>23</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J75" s="2"/>
       <c r="K75" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>108</v>
@@ -5113,7 +5105,7 @@
         <v>604</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>20</v>
@@ -5125,20 +5117,20 @@
         <v>22</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J76" s="2"/>
       <c r="K76" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>173</v>
@@ -5158,7 +5150,7 @@
         <v>605</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>20</v>
@@ -5170,20 +5162,20 @@
         <v>22</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J77" s="2"/>
       <c r="K77" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>173</v>
@@ -5203,7 +5195,7 @@
         <v>608</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>20</v>
@@ -5215,20 +5207,20 @@
         <v>22</v>
       </c>
       <c r="F78" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="H78" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="J78" s="2"/>
       <c r="K78" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>108</v>
@@ -5248,7 +5240,7 @@
         <v>609</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>20</v>
@@ -5260,20 +5252,20 @@
         <v>22</v>
       </c>
       <c r="F79" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G79" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="H79" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>108</v>
@@ -5293,7 +5285,7 @@
         <v>616</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>20</v>
@@ -5305,29 +5297,29 @@
         <v>22</v>
       </c>
       <c r="F80" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="H80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I80" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="J80" s="2"/>
       <c r="K80" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L80" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="N80" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="O80" s="6">
         <v>1</v>
@@ -5338,7 +5330,7 @@
         <v>617</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>20</v>
@@ -5350,29 +5342,29 @@
         <v>22</v>
       </c>
       <c r="F81" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G81" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="H81" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J81" s="2"/>
       <c r="K81" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L81" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="N81" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="M81" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="N81" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="O81" s="6">
         <v>2</v>
@@ -5383,7 +5375,7 @@
         <v>624</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>20</v>
@@ -5395,7 +5387,7 @@
         <v>22</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>102</v>
@@ -5404,11 +5396,11 @@
         <v>3</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J82" s="2"/>
       <c r="K82" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>124</v>
@@ -5428,7 +5420,7 @@
         <v>625</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>20</v>
@@ -5440,7 +5432,7 @@
         <v>22</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>102</v>
@@ -5449,11 +5441,11 @@
         <v>3</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J83" s="2"/>
       <c r="K83" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>124</v>
@@ -5473,7 +5465,7 @@
         <v>628</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>20</v>
@@ -5485,7 +5477,7 @@
         <v>22</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>102</v>
@@ -5494,11 +5486,11 @@
         <v>3</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J84" s="2"/>
       <c r="K84" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>106</v>
@@ -5518,7 +5510,7 @@
         <v>629</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>20</v>
@@ -5530,7 +5522,7 @@
         <v>22</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>102</v>
@@ -5539,11 +5531,11 @@
         <v>3</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J85" s="2"/>
       <c r="K85" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>106</v>
@@ -5563,7 +5555,7 @@
         <v>632</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>20</v>
@@ -5575,20 +5567,20 @@
         <v>22</v>
       </c>
       <c r="F86" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="H86" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="J86" s="2"/>
       <c r="K86" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>106</v>
@@ -5608,7 +5600,7 @@
         <v>633</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>20</v>
@@ -5620,20 +5612,20 @@
         <v>22</v>
       </c>
       <c r="F87" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G87" s="2" t="s">
-        <v>290</v>
-      </c>
       <c r="H87" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>106</v>
@@ -5653,7 +5645,7 @@
         <v>636</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>20</v>
@@ -5665,23 +5657,23 @@
         <v>22</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="J88" s="2"/>
       <c r="K88" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M88" s="2" t="s">
         <v>106</v>
@@ -5698,7 +5690,7 @@
         <v>637</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>20</v>
@@ -5710,23 +5702,23 @@
         <v>22</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J89" s="2"/>
       <c r="K89" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M89" s="2" t="s">
         <v>106</v>
@@ -5743,7 +5735,7 @@
         <v>640</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>20</v>
@@ -5755,7 +5747,7 @@
         <v>22</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>71</v>
@@ -5764,20 +5756,20 @@
         <v>3</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J90" s="2"/>
       <c r="K90" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L90" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="M90" s="2" t="s">
         <v>114</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O90" s="6">
         <v>1</v>
@@ -5788,7 +5780,7 @@
         <v>641</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>20</v>
@@ -5800,7 +5792,7 @@
         <v>22</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>71</v>
@@ -5809,20 +5801,20 @@
         <v>3</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J91" s="2"/>
       <c r="K91" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L91" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="L91" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>114</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O91" s="6">
         <v>0</v>
@@ -5833,7 +5825,7 @@
         <v>644</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>20</v>
@@ -5845,7 +5837,7 @@
         <v>22</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>71</v>
@@ -5854,17 +5846,17 @@
         <v>3</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J92" s="2"/>
       <c r="K92" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L92" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="L92" s="2" t="s">
+      <c r="M92" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="M92" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="N92" s="2" t="s">
         <v>114</v>
@@ -5878,7 +5870,7 @@
         <v>645</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>20</v>
@@ -5890,7 +5882,7 @@
         <v>22</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>71</v>
@@ -5899,17 +5891,17 @@
         <v>3</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J93" s="2"/>
       <c r="K93" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L93" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="L93" s="2" t="s">
+      <c r="M93" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="M93" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>114</v>
@@ -5923,7 +5915,7 @@
         <v>648</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>20</v>
@@ -5935,20 +5927,20 @@
         <v>22</v>
       </c>
       <c r="F94" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G94" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="H94" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="J94" s="2"/>
       <c r="K94" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>108</v>
@@ -5968,7 +5960,7 @@
         <v>649</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>20</v>
@@ -5980,20 +5972,20 @@
         <v>22</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G95" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G95" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="H95" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J95" s="2"/>
       <c r="K95" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>108</v>
@@ -6013,7 +6005,7 @@
         <v>652</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>20</v>
@@ -6025,23 +6017,23 @@
         <v>22</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J96" s="2"/>
       <c r="K96" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M96" s="2" t="s">
         <v>106</v>
@@ -6058,7 +6050,7 @@
         <v>653</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>20</v>
@@ -6070,23 +6062,23 @@
         <v>22</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>106</v>
@@ -6103,7 +6095,7 @@
         <v>656</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>20</v>
@@ -6115,7 +6107,7 @@
         <v>22</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>87</v>
@@ -6124,11 +6116,11 @@
         <v>3</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>108</v>
@@ -6148,7 +6140,7 @@
         <v>657</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>20</v>
@@ -6160,7 +6152,7 @@
         <v>22</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>87</v>
@@ -6169,11 +6161,11 @@
         <v>3</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>108</v>
@@ -6193,7 +6185,7 @@
         <v>660</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>20</v>
@@ -6205,7 +6197,7 @@
         <v>22</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>87</v>
@@ -6214,14 +6206,14 @@
         <v>3</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M100" s="2" t="s">
         <v>108</v>
@@ -6238,7 +6230,7 @@
         <v>661</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>20</v>
@@ -6250,7 +6242,7 @@
         <v>22</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>87</v>
@@ -6259,14 +6251,14 @@
         <v>3</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M101" s="2" t="s">
         <v>108</v>
@@ -6283,7 +6275,7 @@
         <v>664</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>20</v>
@@ -6304,11 +6296,11 @@
         <v>3</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J102" s="2"/>
       <c r="K102" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>106</v>
@@ -6328,7 +6320,7 @@
         <v>665</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>20</v>
@@ -6349,11 +6341,11 @@
         <v>3</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>106</v>
@@ -6373,7 +6365,7 @@
         <v>668</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>20</v>
@@ -6394,17 +6386,17 @@
         <v>3</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J104" s="2"/>
       <c r="K104" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N104" s="2" t="s">
         <v>108</v>
@@ -6418,7 +6410,7 @@
         <v>669</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>20</v>
@@ -6439,17 +6431,17 @@
         <v>3</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J105" s="2"/>
       <c r="K105" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L105" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M105" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>108</v>
@@ -6463,7 +6455,7 @@
         <v>672</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>20</v>
@@ -6475,29 +6467,29 @@
         <v>22</v>
       </c>
       <c r="F106" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G106" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="G106" s="2" t="s">
+      <c r="H106" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I106" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>332</v>
       </c>
       <c r="J106" s="2"/>
       <c r="K106" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>107</v>
       </c>
       <c r="M106" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="N106" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="O106" s="6">
         <v>0</v>
@@ -6508,7 +6500,7 @@
         <v>673</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>20</v>
@@ -6520,29 +6512,29 @@
         <v>22</v>
       </c>
       <c r="F107" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G107" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="G107" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="H107" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J107" s="2"/>
       <c r="K107" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>107</v>
       </c>
       <c r="M107" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="N107" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="O107" s="6">
         <v>2</v>
@@ -6553,7 +6545,7 @@
         <v>676</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>20</v>
@@ -6565,29 +6557,29 @@
         <v>22</v>
       </c>
       <c r="F108" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I108" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="J108" s="2"/>
       <c r="K108" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>131</v>
       </c>
       <c r="M108" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O108" s="6">
         <v>0</v>
@@ -6598,7 +6590,7 @@
         <v>677</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>20</v>
@@ -6610,29 +6602,29 @@
         <v>22</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H109" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I109" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="J109" s="2"/>
       <c r="K109" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>131</v>
       </c>
       <c r="M109" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O109" s="6">
         <v>2</v>
@@ -6643,7 +6635,7 @@
         <v>872</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>20</v>
@@ -6655,29 +6647,29 @@
         <v>22</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I110" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="J110" s="2"/>
       <c r="K110" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="M110" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="L110" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="M110" s="2" t="s">
+      <c r="N110" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="N110" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="O110" s="6">
         <v>0</v>
@@ -6688,7 +6680,7 @@
         <v>873</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>20</v>
@@ -6700,29 +6692,29 @@
         <v>22</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H111" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J111" s="2"/>
       <c r="K111" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="M111" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="L111" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="M111" s="2" t="s">
+      <c r="N111" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="N111" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="O111" s="6">
         <v>2</v>
@@ -6733,7 +6725,7 @@
         <v>1068</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>20</v>
@@ -6745,29 +6737,29 @@
         <v>22</v>
       </c>
       <c r="F112" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I112" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H112" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I112" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="J112" s="2"/>
       <c r="K112" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M112" s="2" t="s">
         <v>143</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O112" s="6">
         <v>1</v>
@@ -6778,7 +6770,7 @@
         <v>1069</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>20</v>
@@ -6790,29 +6782,29 @@
         <v>22</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H113" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J113" s="2"/>
       <c r="K113" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M113" s="2" t="s">
         <v>143</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O113" s="6">
         <v>2</v>
@@ -6823,7 +6815,7 @@
         <v>1072</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>20</v>
@@ -6835,29 +6827,29 @@
         <v>22</v>
       </c>
       <c r="F114" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I114" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="G114" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H114" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>355</v>
       </c>
       <c r="J114" s="2"/>
       <c r="K114" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="L114" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="M114" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="L114" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="M114" s="2" t="s">
+      <c r="N114" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="N114" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="O114" s="6">
         <v>0</v>
@@ -6868,7 +6860,7 @@
         <v>1073</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>20</v>
@@ -6880,29 +6872,29 @@
         <v>22</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J115" s="2"/>
       <c r="K115" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="M115" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="L115" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="M115" s="2" t="s">
+      <c r="N115" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="N115" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="O115" s="6">
         <v>2</v>
@@ -6913,7 +6905,7 @@
         <v>1268</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>20</v>
@@ -6925,26 +6917,26 @@
         <v>22</v>
       </c>
       <c r="F116" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I116" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>361</v>
       </c>
       <c r="J116" s="2"/>
       <c r="K116" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M116" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>173</v>
@@ -6958,7 +6950,7 @@
         <v>1269</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>20</v>
@@ -6970,26 +6962,26 @@
         <v>22</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J117" s="2"/>
       <c r="K117" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L117" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M117" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>173</v>
@@ -7003,7 +6995,7 @@
         <v>1272</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>20</v>
@@ -7015,29 +7007,29 @@
         <v>22</v>
       </c>
       <c r="F118" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G118" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="H118" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I118" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="J118" s="2"/>
       <c r="K118" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M118" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L118" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="M118" s="2" t="s">
+      <c r="N118" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="N118" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="O118" s="6">
         <v>0</v>
@@ -7048,7 +7040,7 @@
         <v>1273</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>20</v>
@@ -7060,29 +7052,29 @@
         <v>22</v>
       </c>
       <c r="F119" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G119" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="G119" s="2" t="s">
-        <v>366</v>
-      </c>
       <c r="H119" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J119" s="2"/>
       <c r="K119" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M119" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L119" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="M119" s="2" t="s">
+      <c r="N119" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="N119" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="O119" s="6">
         <v>2</v>
@@ -7093,7 +7085,7 @@
         <v>1344</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>20</v>
@@ -7105,26 +7097,26 @@
         <v>22</v>
       </c>
       <c r="F120" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I120" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I120" s="2" t="s">
-        <v>373</v>
       </c>
       <c r="J120" s="2"/>
       <c r="K120" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M120" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>166</v>
@@ -7138,7 +7130,7 @@
         <v>1345</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>20</v>
@@ -7150,26 +7142,26 @@
         <v>22</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J121" s="2"/>
       <c r="K121" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M121" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>166</v>
@@ -7183,7 +7175,7 @@
         <v>1472</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>20</v>
@@ -7195,29 +7187,29 @@
         <v>22</v>
       </c>
       <c r="F122" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G122" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="H122" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I122" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I122" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="J122" s="2"/>
       <c r="K122" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M122" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O122" s="6">
         <v>0</v>
@@ -7228,7 +7220,7 @@
         <v>1473</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>20</v>
@@ -7240,29 +7232,29 @@
         <v>22</v>
       </c>
       <c r="F123" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G123" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="G123" s="2" t="s">
-        <v>378</v>
-      </c>
       <c r="H123" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J123" s="2"/>
       <c r="K123" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L123" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M123" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O123" s="6">
         <v>1</v>
@@ -7273,7 +7265,7 @@
         <v>1536</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>20</v>
@@ -7285,26 +7277,26 @@
         <v>22</v>
       </c>
       <c r="F124" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I124" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="G124" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I124" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="J124" s="2"/>
       <c r="K124" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M124" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N124" s="2" t="s">
         <v>124</v>
@@ -7318,7 +7310,7 @@
         <v>1537</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>20</v>
@@ -7330,26 +7322,26 @@
         <v>22</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J125" s="2"/>
       <c r="K125" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>124</v>
@@ -7363,7 +7355,7 @@
         <v>1672</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>20</v>
@@ -7375,29 +7367,29 @@
         <v>22</v>
       </c>
       <c r="F126" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G126" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="H126" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I126" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I126" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="J126" s="2"/>
       <c r="K126" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M126" s="2" t="s">
         <v>131</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O126" s="6">
         <v>1</v>
@@ -7408,7 +7400,7 @@
         <v>1673</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>20</v>
@@ -7420,29 +7412,29 @@
         <v>22</v>
       </c>
       <c r="F127" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G127" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G127" s="2" t="s">
-        <v>389</v>
-      </c>
       <c r="H127" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J127" s="2"/>
       <c r="K127" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M127" s="2" t="s">
         <v>131</v>
       </c>
       <c r="N127" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O127" s="6">
         <v>2</v>
@@ -7453,7 +7445,7 @@
         <v>1720</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>20</v>
@@ -7465,29 +7457,29 @@
         <v>22</v>
       </c>
       <c r="F128" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I128" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="G128" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I128" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="J128" s="2"/>
       <c r="K128" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M128" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N128" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O128" s="6">
         <v>1</v>
@@ -7498,7 +7490,7 @@
         <v>1872</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>20</v>
@@ -7510,29 +7502,29 @@
         <v>22</v>
       </c>
       <c r="F129" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G129" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="H129" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I129" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="H129" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I129" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="J129" s="2"/>
       <c r="K129" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="L129" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="L129" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="M129" s="2" t="s">
         <v>166</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O129" s="6">
         <v>1</v>
@@ -7543,7 +7535,7 @@
         <v>1873</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>20</v>
@@ -7555,29 +7547,29 @@
         <v>22</v>
       </c>
       <c r="F130" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G130" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="G130" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="H130" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J130" s="2"/>
       <c r="K130" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="L130" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="L130" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="M130" s="2" t="s">
         <v>166</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O130" s="6">
         <v>2</v>

</xml_diff>